<commit_message>
Added more images to expand ther dataset, succesfully building the test and training sets.
</commit_message>
<xml_diff>
--- a/DataSetImagesIds.xlsx
+++ b/DataSetImagesIds.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JPData\UNCC\ITCS-5154\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JPData\UNCC\ITCS-5154\Project\ProjectCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{435B0C48-CAD8-46F4-91E9-5AE20C248987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55DE3B5-88BA-4872-BCA7-F1B2843467E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8070" yWindow="6000" windowWidth="23220" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14985" yWindow="5940" windowWidth="23220" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="26">
   <si>
     <t>Unit Name</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Infernus Marine</t>
   </si>
   <si>
-    <t xml:space="preserve">Brutalis Dreadnought </t>
-  </si>
-  <si>
     <t>Assault Intercessor With Jump Pack</t>
   </si>
   <si>
@@ -103,6 +100,9 @@
   </si>
   <si>
     <t>Image ID</t>
+  </si>
+  <si>
+    <t>Brutalis Dreadnought</t>
   </si>
 </sst>
 </file>
@@ -420,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,7 +434,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -557,7 +557,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -565,7 +565,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -573,7 +573,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -581,7 +581,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -597,7 +597,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -605,7 +605,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -613,7 +613,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -621,7 +621,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -629,7 +629,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -637,7 +637,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -645,7 +645,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -653,7 +653,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -661,7 +661,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -669,7 +669,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -677,7 +677,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -685,7 +685,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -701,7 +701,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -725,7 +725,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -733,7 +733,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -741,7 +741,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -749,7 +749,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -757,7 +757,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -765,7 +765,311 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more images to the dataset and introduced two new units to classify by.
</commit_message>
<xml_diff>
--- a/DataSetImagesIds.xlsx
+++ b/DataSetImagesIds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JPData\UNCC\ITCS-5154\Project\ProjectCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55DE3B5-88BA-4872-BCA7-F1B2843467E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1AA8286-70EE-4DED-A141-591FD9644307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14985" yWindow="5940" windowWidth="23220" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20700" yWindow="3480" windowWidth="23220" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="28">
   <si>
     <t>Unit Name</t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t>Brutalis Dreadnought</t>
+  </si>
+  <si>
+    <t>Apothecary</t>
+  </si>
+  <si>
+    <t>Ballistus Dreadnought</t>
   </si>
 </sst>
 </file>
@@ -420,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B80"/>
+  <dimension ref="A1:B124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E81" sqref="E81"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="E127" sqref="E127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,6 +1078,358 @@
         <v>15</v>
       </c>
     </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="B103" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="B104" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>104</v>
+      </c>
+      <c r="B105" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>105</v>
+      </c>
+      <c r="B106" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>106</v>
+      </c>
+      <c r="B107" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>107</v>
+      </c>
+      <c r="B108" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>108</v>
+      </c>
+      <c r="B109" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>109</v>
+      </c>
+      <c r="B110" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>110</v>
+      </c>
+      <c r="B111" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>111</v>
+      </c>
+      <c r="B112" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>112</v>
+      </c>
+      <c r="B113" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>113</v>
+      </c>
+      <c r="B114" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>114</v>
+      </c>
+      <c r="B115" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>115</v>
+      </c>
+      <c r="B116" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>116</v>
+      </c>
+      <c r="B117" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>117</v>
+      </c>
+      <c r="B118" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>118</v>
+      </c>
+      <c r="B119" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>119</v>
+      </c>
+      <c r="B120" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>120</v>
+      </c>
+      <c r="B121" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>121</v>
+      </c>
+      <c r="B122" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>122</v>
+      </c>
+      <c r="B123" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>123</v>
+      </c>
+      <c r="B124" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Completed the current dataset to use for the project. Converted images to BW, and added the testing set.
</commit_message>
<xml_diff>
--- a/DataSetImagesIds.xlsx
+++ b/DataSetImagesIds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JPData\UNCC\ITCS-5154\Project\ProjectCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1AA8286-70EE-4DED-A141-591FD9644307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6186AB0-D757-401D-ACA7-77A0919A4219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20700" yWindow="3480" windowWidth="23220" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15735" yWindow="6240" windowWidth="23220" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="28">
   <si>
     <t>Unit Name</t>
   </si>
@@ -426,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B124"/>
+  <dimension ref="A1:B161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="E127" sqref="E127"/>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="C159" sqref="C159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1430,6 +1430,302 @@
         <v>26</v>
       </c>
     </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>124</v>
+      </c>
+      <c r="B125" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>125</v>
+      </c>
+      <c r="B126" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>126</v>
+      </c>
+      <c r="B127" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>127</v>
+      </c>
+      <c r="B128" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>128</v>
+      </c>
+      <c r="B129" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>129</v>
+      </c>
+      <c r="B130" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>130</v>
+      </c>
+      <c r="B131" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>131</v>
+      </c>
+      <c r="B132" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>132</v>
+      </c>
+      <c r="B133" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>133</v>
+      </c>
+      <c r="B134" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>134</v>
+      </c>
+      <c r="B135" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>135</v>
+      </c>
+      <c r="B136" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>136</v>
+      </c>
+      <c r="B137" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>137</v>
+      </c>
+      <c r="B138" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>138</v>
+      </c>
+      <c r="B139" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>139</v>
+      </c>
+      <c r="B140" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>140</v>
+      </c>
+      <c r="B141" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>141</v>
+      </c>
+      <c r="B142" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>142</v>
+      </c>
+      <c r="B143" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>143</v>
+      </c>
+      <c r="B144" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>144</v>
+      </c>
+      <c r="B145" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>145</v>
+      </c>
+      <c r="B146" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>146</v>
+      </c>
+      <c r="B147" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>147</v>
+      </c>
+      <c r="B148" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>148</v>
+      </c>
+      <c r="B149" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>149</v>
+      </c>
+      <c r="B150" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>150</v>
+      </c>
+      <c r="B151" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>151</v>
+      </c>
+      <c r="B152" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>152</v>
+      </c>
+      <c r="B153" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>153</v>
+      </c>
+      <c r="B154" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>154</v>
+      </c>
+      <c r="B155" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>155</v>
+      </c>
+      <c r="B156" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>156</v>
+      </c>
+      <c r="B157" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>157</v>
+      </c>
+      <c r="B158" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>158</v>
+      </c>
+      <c r="B159" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>159</v>
+      </c>
+      <c r="B160" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>160</v>
+      </c>
+      <c r="B161" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>